<commit_message>
sot ngay cong cuong
</commit_message>
<xml_diff>
--- a/Data/062018/phancong.xlsx
+++ b/Data/062018/phancong.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{F354918C-3C3E-4F2F-8A6D-770288928455}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03781724-C9A1-4058-8E7F-7A821A0DD138}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7695" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="20">
   <si>
     <t>x01593</t>
   </si>
@@ -436,10 +436,10 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D31" sqref="D31"/>
+      <selection pane="bottomRight" activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -792,6 +792,9 @@
       <c r="A27" s="3">
         <v>43277</v>
       </c>
+      <c r="B27" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>

</xml_diff>